<commit_message>
New words had been added
</commit_message>
<xml_diff>
--- a/data/reword.xlsx
+++ b/data/reword.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Python-Rush\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PythonProjects\MicroProjects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F459EB80-75C4-4766-ABD0-61F392B0552C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9DBC93-26A3-4696-99D2-7954AA112D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3444" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13365" yWindow="1545" windowWidth="14280" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
   <si>
     <t>English</t>
   </si>
@@ -397,6 +397,150 @@
   </si>
   <si>
     <t>ссориться</t>
+  </si>
+  <si>
+    <t>gotta (I have got to)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">мне нужно, я вынужден </t>
+  </si>
+  <si>
+    <t>to part ways</t>
+  </si>
+  <si>
+    <t>Закончиться, разойтись, расстаться</t>
+  </si>
+  <si>
+    <t>sick and tired</t>
+  </si>
+  <si>
+    <t>Mockingjay</t>
+  </si>
+  <si>
+    <t>сойка-пересмешника</t>
+  </si>
+  <si>
+    <t>Откровенно достало</t>
+  </si>
+  <si>
+    <t>застегнуть (ремень)</t>
+  </si>
+  <si>
+    <t>Застегнуть молнию</t>
+  </si>
+  <si>
+    <t>to twist</t>
+  </si>
+  <si>
+    <t>сделать человеку плохо</t>
+  </si>
+  <si>
+    <t>to fasten</t>
+  </si>
+  <si>
+    <t>to zip</t>
+  </si>
+  <si>
+    <t>Притормозить (про человека)</t>
+  </si>
+  <si>
+    <t>to let up</t>
+  </si>
+  <si>
+    <t>Ослабевать, сходить на нет</t>
+  </si>
+  <si>
+    <t>to slow up (down)</t>
+  </si>
+  <si>
+    <t>sacrilegious</t>
+  </si>
+  <si>
+    <t>кощунственный</t>
+  </si>
+  <si>
+    <t>take forever</t>
+  </si>
+  <si>
+    <t>Очень долго (время)</t>
+  </si>
+  <si>
+    <t>run-in</t>
+  </si>
+  <si>
+    <t>схватка</t>
+  </si>
+  <si>
+    <t>to detract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уменьшать </t>
+  </si>
+  <si>
+    <t>detractors</t>
+  </si>
+  <si>
+    <t>недоброжелатели</t>
+  </si>
+  <si>
+    <t>pitchfork</t>
+  </si>
+  <si>
+    <t>вилы</t>
+  </si>
+  <si>
+    <t>corkscrew</t>
+  </si>
+  <si>
+    <t>штопор</t>
+  </si>
+  <si>
+    <t>revenge</t>
+  </si>
+  <si>
+    <t>расплата, месть</t>
+  </si>
+  <si>
+    <t>leeches</t>
+  </si>
+  <si>
+    <t>пиявки</t>
+  </si>
+  <si>
+    <t>flip the bird</t>
+  </si>
+  <si>
+    <t>Поднять средний палец</t>
+  </si>
+  <si>
+    <t>Lip-syncs</t>
+  </si>
+  <si>
+    <t>Липсинг</t>
+  </si>
+  <si>
+    <t>hardly</t>
+  </si>
+  <si>
+    <t>Едва ли</t>
+  </si>
+  <si>
+    <t>prolly</t>
+  </si>
+  <si>
+    <t>возможно (prodadly)</t>
+  </si>
+  <si>
+    <t>to fetch</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>пульт</t>
+  </si>
+  <si>
+    <t>пойди принеси (часто говорят собакам)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -714,18 +858,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C65"/>
+  <dimension ref="B3:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -733,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -741,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>98</v>
       </c>
@@ -749,7 +894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>99</v>
       </c>
@@ -757,7 +902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -765,7 +910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -773,7 +918,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -781,7 +926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>96</v>
       </c>
@@ -789,7 +934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -797,7 +942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -805,7 +950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>95</v>
       </c>
@@ -813,7 +958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -821,7 +966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -829,7 +974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -837,7 +982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -845,7 +990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -853,7 +998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -861,7 +1006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -869,7 +1014,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -877,7 +1022,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -885,7 +1030,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -893,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>36</v>
       </c>
@@ -901,7 +1046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -909,7 +1054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -917,7 +1062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -925,7 +1070,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>43</v>
       </c>
@@ -933,7 +1078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>45</v>
       </c>
@@ -941,7 +1086,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>47</v>
       </c>
@@ -949,7 +1094,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>48</v>
       </c>
@@ -957,7 +1102,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>51</v>
       </c>
@@ -965,7 +1110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>94</v>
       </c>
@@ -973,7 +1118,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>93</v>
       </c>
@@ -981,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>55</v>
       </c>
@@ -989,7 +1134,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>57</v>
       </c>
@@ -997,7 +1142,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>59</v>
       </c>
@@ -1005,7 +1150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>61</v>
       </c>
@@ -1013,7 +1158,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>63</v>
       </c>
@@ -1021,7 +1166,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>65</v>
       </c>
@@ -1029,7 +1174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>67</v>
       </c>
@@ -1037,7 +1182,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>69</v>
       </c>
@@ -1045,7 +1190,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>71</v>
       </c>
@@ -1053,7 +1198,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>73</v>
       </c>
@@ -1061,7 +1206,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>91</v>
       </c>
@@ -1069,7 +1214,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>92</v>
       </c>
@@ -1077,7 +1222,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -1085,7 +1230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>89</v>
       </c>
@@ -1093,7 +1238,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>88</v>
       </c>
@@ -1101,7 +1246,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>80</v>
       </c>
@@ -1109,7 +1254,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>82</v>
       </c>
@@ -1117,7 +1262,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>84</v>
       </c>
@@ -1125,7 +1270,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>86</v>
       </c>
@@ -1133,7 +1278,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>100</v>
       </c>
@@ -1141,7 +1286,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>102</v>
       </c>
@@ -1149,7 +1294,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>104</v>
       </c>
@@ -1157,7 +1302,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>106</v>
       </c>
@@ -1165,7 +1310,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>108</v>
       </c>
@@ -1173,7 +1318,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>110</v>
       </c>
@@ -1181,7 +1326,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>112</v>
       </c>
@@ -1189,7 +1334,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>116</v>
       </c>
@@ -1197,7 +1342,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>114</v>
       </c>
@@ -1205,7 +1350,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>118</v>
       </c>
@@ -1213,7 +1358,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>120</v>
       </c>
@@ -1221,12 +1366,204 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>139</v>
+      </c>
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+      <c r="C76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>158</v>
+      </c>
+      <c r="C83" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>